<commit_message>
MAJ Rapport et schemas-blocs
</commit_message>
<xml_diff>
--- a/doc/planification/2312_BadgePlace_Journal.xlsx
+++ b/doc/planification/2312_BadgePlace_Journal.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -51,6 +51,29 @@
   </si>
   <si>
     <t>Le choix de réalisé Le module soit-même demande des compétences dans Le design des antennes</t>
+  </si>
+  <si>
+    <t>08:30 - 10:00</t>
+  </si>
+  <si>
+    <t>Schéma bloc de principe</t>
+  </si>
+  <si>
+    <t>Recherche des composants à utiliser :
+- Module RFID
+- Convertisseur AC/DC
+- Relais de commutation
+- Gestion de la base de donnée
+- Boitier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation des composants :
+- Module RFID = MIKROE-1434
+- Convertisseur AC/DC = RAC03-3.3SK
+</t>
+  </si>
+  <si>
+    <t>12:30 - 16:00</t>
   </si>
 </sst>
 </file>
@@ -94,14 +117,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -383,16 +406,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12" style="2" customWidth="1"/>
-    <col min="3" max="3" width="29" style="5" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="4" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="11.42578125" style="1"/>
   </cols>
@@ -404,7 +427,7 @@
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -412,28 +435,62 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="5">
         <v>45159</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>45160</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Journal de travail + MAJ Altium
</commit_message>
<xml_diff>
--- a/doc/planification/2312_BadgePlace_Journal.xlsx
+++ b/doc/planification/2312_BadgePlace_Journal.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migsantos\MIGSAN_GIT\2312_BadgePlace\doc\planification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ETML-ES\2312_BadgePlace\doc\planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B005058-7CF2-484A-BE11-4E2EF19D9F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -111,11 +112,33 @@
   <si>
     <t>08:00 - 10:30</t>
   </si>
+  <si>
+    <t>10:30 - 11:00</t>
+  </si>
+  <si>
+    <t>Trop de composants externe, le prix final revient au même que les modules concurrents</t>
+  </si>
+  <si>
+    <t>Recherche et choix d'un nouveau convertisseur AC/DC : Traco TMPW_5-103
+Offre plus de protections, de meilleures certifications EMC, le tout en un seul bloc sans composants externes, entreprise et fabrication Suisse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:00 - 16:00 </t>
+  </si>
+  <si>
+    <t>Début de la schématique d'alimentation, recherche des symboles et footprints des composants.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:00 - 17:00 </t>
+  </si>
+  <si>
+    <t>Organisation du projet. Ecriture du rapport.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -145,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -158,9 +181,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -444,14 +464,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,8 +497,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>45159</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -488,8 +508,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -501,7 +521,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>45160</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -511,8 +531,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+    <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -520,8 +540,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
@@ -529,8 +549,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+    <row r="7" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>45161</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -540,8 +560,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
       <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
@@ -549,8 +569,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
@@ -558,8 +578,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
@@ -567,7 +587,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>45162</v>
       </c>
@@ -577,12 +597,43 @@
       <c r="C11" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="D11" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalisation de la schématique ETHERNET
</commit_message>
<xml_diff>
--- a/doc/planification/2312_BadgePlace_Journal.xlsx
+++ b/doc/planification/2312_BadgePlace_Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ETML-ES\2312_BadgePlace\doc\planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B005058-7CF2-484A-BE11-4E2EF19D9F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9991B39-E6D2-4B61-A16C-D78910790032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Recherche sur le module WIFI et le module ethernet</t>
   </si>
   <si>
-    <t>Rendez-vous avec maitre de diplôme</t>
-  </si>
-  <si>
     <t>14:00 - 16:30</t>
   </si>
   <si>
@@ -133,6 +130,36 @@
   </si>
   <si>
     <t>Organisation du projet. Ecriture du rapport.</t>
+  </si>
+  <si>
+    <t>Séance avec maitre de diplôme</t>
+  </si>
+  <si>
+    <t>08:00 - 10:00</t>
+  </si>
+  <si>
+    <t>Séance hebdomadaire avec maître de diplôme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00 - 12:00 </t>
+  </si>
+  <si>
+    <t>Rédaction du procés-verbal de la séance hebdomadaire</t>
+  </si>
+  <si>
+    <t>16:00 - 17:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réalisation de tests sur la consommation de courant des différents appareils. </t>
+  </si>
+  <si>
+    <t>Réalisation de la schématique, recherches de footprints et de composants.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00 - 16:00 </t>
+  </si>
+  <si>
+    <t>Réalisation la schématique du connecteur et contrôleur Ethernet. Recherche du fonctionnement et des footprints des composants nécessaires</t>
   </si>
 </sst>
 </file>
@@ -168,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -181,6 +208,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -468,10 +498,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +528,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <v>45159</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -509,7 +539,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -521,7 +551,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="6">
         <v>45160</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -532,7 +562,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -541,7 +571,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
@@ -550,7 +580,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="6">
         <v>45161</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -561,7 +591,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
@@ -570,70 +600,120 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>45162</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>45162</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="D11" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="4" t="s">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="4" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>30</v>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>45163</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>45164</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Fin de séance d'écriture du rapport
</commit_message>
<xml_diff>
--- a/doc/planification/2312_BadgePlace_Journal.xlsx
+++ b/doc/planification/2312_BadgePlace_Journal.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -299,6 +299,13 @@
   <si>
     <t>Mise à jours du planning (pour inclure week-ends et décallage)
 Rédaction et envoi du PV.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rédaction de la partie "Design" du rapport
+Mise en page générale </t>
+  </si>
+  <si>
+    <t>13:30 - 17:00</t>
   </si>
 </sst>
 </file>
@@ -334,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -359,6 +366,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,10 +653,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,18 +1105,38 @@
         <v>83</v>
       </c>
     </row>
+    <row r="45" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
+        <v>45174</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="8"/>
+      <c r="B46" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A40:A44"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="A21:A26"/>
     <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Début de la programmation UART
</commit_message>
<xml_diff>
--- a/doc/planification/2312_BadgePlace_Journal.xlsx
+++ b/doc/planification/2312_BadgePlace_Journal.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
   <si>
     <t>Date</t>
   </si>
@@ -306,6 +306,22 @@
   </si>
   <si>
     <t>13:30 - 17:00</t>
+  </si>
+  <si>
+    <t>08:30 - 10:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réalisation d'un câble pour le module RFID </t>
+  </si>
+  <si>
+    <t>Pas la bonne pince à sertir pour le connecteur. -&gt; Commande d'un cable pré-monté</t>
+  </si>
+  <si>
+    <t>10:30 - 11:30</t>
+  </si>
+  <si>
+    <t>Configuration du projet Harmony sur MPLAB
+et récupération des librairies nécessaires au projet</t>
   </si>
 </sst>
 </file>
@@ -341,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -369,6 +385,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -653,9 +672,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
@@ -683,7 +702,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="10">
         <v>45159</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -694,7 +713,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -706,7 +725,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="10">
         <v>45160</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -717,7 +736,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -726,7 +745,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
@@ -735,7 +754,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="10">
         <v>45161</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -746,7 +765,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="10"/>
       <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
@@ -755,7 +774,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
@@ -764,7 +783,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
@@ -773,7 +792,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="10">
         <v>45162</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -787,7 +806,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
@@ -796,7 +815,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
@@ -805,7 +824,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="2" t="s">
         <v>28</v>
       </c>
@@ -814,7 +833,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="10">
         <v>45163</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -825,7 +844,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
@@ -834,7 +853,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
@@ -843,7 +862,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
@@ -874,7 +893,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="A21" s="10">
         <v>45166</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -885,7 +904,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="6" t="s">
         <v>44</v>
       </c>
@@ -894,7 +913,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="6" t="s">
         <v>45</v>
       </c>
@@ -903,7 +922,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="2" t="s">
         <v>46</v>
       </c>
@@ -912,7 +931,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="2" t="s">
         <v>49</v>
       </c>
@@ -921,7 +940,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+      <c r="A26" s="10"/>
       <c r="B26" s="2" t="s">
         <v>51</v>
       </c>
@@ -930,7 +949,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
+      <c r="A27" s="10">
         <v>45167</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -941,7 +960,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="2" t="s">
         <v>55</v>
       </c>
@@ -950,7 +969,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+      <c r="A29" s="10"/>
       <c r="B29" s="2" t="s">
         <v>58</v>
       </c>
@@ -959,7 +978,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
+      <c r="A30" s="10">
         <v>45168</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -970,7 +989,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
+      <c r="A31" s="10"/>
       <c r="B31" s="2" t="s">
         <v>59</v>
       </c>
@@ -979,7 +998,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
+      <c r="A32" s="10"/>
       <c r="B32" s="2" t="s">
         <v>61</v>
       </c>
@@ -987,8 +1006,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
       <c r="B33" s="2" t="s">
         <v>64</v>
       </c>
@@ -996,7 +1015,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>45169</v>
       </c>
@@ -1007,7 +1026,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>45170</v>
       </c>
@@ -1018,7 +1037,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>45171</v>
       </c>
@@ -1029,8 +1048,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="8">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
         <v>45172</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1040,8 +1059,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
       <c r="B38" s="2" t="s">
         <v>73</v>
       </c>
@@ -1049,8 +1068,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
       <c r="B39" s="2" t="s">
         <v>74</v>
       </c>
@@ -1058,8 +1077,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="8">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
         <v>45173</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -1069,8 +1088,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
       <c r="B41" s="2" t="s">
         <v>4</v>
       </c>
@@ -1078,8 +1097,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
       <c r="B42" s="6" t="s">
         <v>78</v>
       </c>
@@ -1087,8 +1106,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
       <c r="B43" s="2" t="s">
         <v>80</v>
       </c>
@@ -1096,8 +1115,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
       <c r="B44" s="2" t="s">
         <v>82</v>
       </c>
@@ -1105,8 +1124,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="8">
+    <row r="45" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="10">
         <v>45174</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -1116,12 +1135,34 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
       <c r="B46" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C46" s="9"/>
+    </row>
+    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="8">
+        <v>45175</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
Fin de sessions de prog et rapport
</commit_message>
<xml_diff>
--- a/doc/planification/2312_BadgePlace_Journal.xlsx
+++ b/doc/planification/2312_BadgePlace_Journal.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="94">
   <si>
     <t>Date</t>
   </si>
@@ -322,6 +322,15 @@
   <si>
     <t>Configuration du projet Harmony sur MPLAB
 et récupération des librairies nécessaires au projet</t>
+  </si>
+  <si>
+    <t>13:30 - 20:00</t>
+  </si>
+  <si>
+    <t>Lecture de la documentation et programmation du module RFID "CHILLI"</t>
+  </si>
+  <si>
+    <t>Programmation du module RFID "CHILLI" avec utilisation des librairies du fabricant</t>
   </si>
 </sst>
 </file>
@@ -380,13 +389,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -672,10 +681,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,7 +711,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="9">
         <v>45159</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -713,7 +722,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -725,7 +734,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <v>45160</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -736,7 +745,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -745,7 +754,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
@@ -754,7 +763,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>45161</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -765,7 +774,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
@@ -774,7 +783,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
@@ -783,7 +792,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
@@ -792,7 +801,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="A11" s="9">
         <v>45162</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -806,7 +815,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
@@ -815,7 +824,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
@@ -824,7 +833,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="2" t="s">
         <v>28</v>
       </c>
@@ -833,7 +842,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="A15" s="9">
         <v>45163</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -844,7 +853,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
@@ -853,7 +862,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
@@ -862,7 +871,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
@@ -893,7 +902,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
+      <c r="A21" s="9">
         <v>45166</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -904,7 +913,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="6" t="s">
         <v>44</v>
       </c>
@@ -913,7 +922,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="6" t="s">
         <v>45</v>
       </c>
@@ -922,7 +931,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
+      <c r="A24" s="9"/>
       <c r="B24" s="2" t="s">
         <v>46</v>
       </c>
@@ -931,7 +940,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="2" t="s">
         <v>49</v>
       </c>
@@ -940,7 +949,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="2" t="s">
         <v>51</v>
       </c>
@@ -949,7 +958,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
+      <c r="A27" s="9">
         <v>45167</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -960,7 +969,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="2" t="s">
         <v>55</v>
       </c>
@@ -969,7 +978,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="2" t="s">
         <v>58</v>
       </c>
@@ -978,7 +987,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
+      <c r="A30" s="9">
         <v>45168</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -989,7 +998,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="2" t="s">
         <v>59</v>
       </c>
@@ -998,7 +1007,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="2" t="s">
         <v>61</v>
       </c>
@@ -1007,7 +1016,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="2" t="s">
         <v>64</v>
       </c>
@@ -1049,7 +1058,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="10">
+      <c r="A37" s="9">
         <v>45172</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1060,7 +1069,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
+      <c r="A38" s="9"/>
       <c r="B38" s="2" t="s">
         <v>73</v>
       </c>
@@ -1069,7 +1078,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="2" t="s">
         <v>74</v>
       </c>
@@ -1078,7 +1087,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="10">
+      <c r="A40" s="9">
         <v>45173</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -1089,7 +1098,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
+      <c r="A41" s="9"/>
       <c r="B41" s="2" t="s">
         <v>4</v>
       </c>
@@ -1098,7 +1107,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
+      <c r="A42" s="9"/>
       <c r="B42" s="6" t="s">
         <v>78</v>
       </c>
@@ -1107,7 +1116,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
+      <c r="A43" s="9"/>
       <c r="B43" s="2" t="s">
         <v>80</v>
       </c>
@@ -1116,7 +1125,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
+      <c r="A44" s="9"/>
       <c r="B44" s="2" t="s">
         <v>82</v>
       </c>
@@ -1125,25 +1134,25 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="10">
+      <c r="A45" s="9">
         <v>45174</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="8" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
+      <c r="A46" s="9"/>
       <c r="B46" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C46" s="9"/>
+      <c r="C46" s="8"/>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="8">
+      <c r="A47" s="9">
         <v>45175</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -1157,6 +1166,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="9"/>
       <c r="B48" s="2" t="s">
         <v>89</v>
       </c>
@@ -1164,8 +1174,38 @@
         <v>90</v>
       </c>
     </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="9"/>
+      <c r="B49" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="9">
+        <v>45176</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
+      <c r="B51" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="15">
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="A50:A51"/>
     <mergeCell ref="C45:C46"/>
     <mergeCell ref="A45:A46"/>
     <mergeCell ref="A2:A3"/>

</xml_diff>

<commit_message>
Fin de la troisième semaine !
</commit_message>
<xml_diff>
--- a/doc/planification/2312_BadgePlace_Journal.xlsx
+++ b/doc/planification/2312_BadgePlace_Journal.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="100">
   <si>
     <t>Date</t>
   </si>
@@ -336,7 +336,19 @@
     <t>17:00 - 19:00</t>
   </si>
   <si>
-    <t>Rédaction de rapport</t>
+    <t>Rédaction de rapport (design)</t>
+  </si>
+  <si>
+    <t>Rédaction de rapport (page de titre + design)</t>
+  </si>
+  <si>
+    <t>11:30 - 12:30</t>
+  </si>
+  <si>
+    <t>13:30 - 16:00</t>
+  </si>
+  <si>
+    <t>Programmation module RFID</t>
   </si>
 </sst>
 </file>
@@ -684,10 +696,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,26 +1222,56 @@
         <v>94</v>
       </c>
       <c r="C52" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="8">
+        <v>45177</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>95</v>
       </c>
     </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="8"/>
+      <c r="B54" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="8"/>
+      <c r="B55" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A40:A44"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="A21:A26"/>
     <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A50:A52"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Remise du rapport final
</commit_message>
<xml_diff>
--- a/doc/planification/2312_BadgePlace_Journal.xlsx
+++ b/doc/planification/2312_BadgePlace_Journal.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ETML-ES\2312_BadgePlace\doc\planification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\microchip\harmony\v2_06\apps\2312_BadgePlace\doc\planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B596DB-B02E-4A3B-A4B3-AFE2B6D4040C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="136">
   <si>
     <t>Date</t>
   </si>
@@ -395,16 +394,10 @@
     <t>Semaine 4</t>
   </si>
   <si>
-    <t>Journal de travail</t>
-  </si>
-  <si>
     <t>Semaine 5</t>
   </si>
   <si>
     <t>Semaine 6</t>
-  </si>
-  <si>
-    <t>Semaine 7</t>
   </si>
   <si>
     <t>Réalisation des librairies de contrôle des LEDS</t>
@@ -456,12 +449,29 @@
   <si>
     <t>Programmation de l'ESP32 avec connexion Wi-Fi.
 Mise à jours de divers documents annexes</t>
+  </si>
+  <si>
+    <t>Programmation du module RFID et ESP32 + autres machines d'états</t>
+  </si>
+  <si>
+    <t>08:00 - 00:00</t>
+  </si>
+  <si>
+    <t>Rédaction du rapport et de la documentation</t>
+  </si>
+  <si>
+    <t>10:00 - 00:00</t>
+  </si>
+  <si>
+    <t>2312 Badge pour place de travail
+Miguel Santos
+Journal de travail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -790,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -871,15 +881,51 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -889,46 +935,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1209,14 +1225,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,12 +1243,12 @@
     <col min="5" max="16384" width="0.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
@@ -1246,14 +1262,14 @@
       </c>
     </row>
     <row r="3" spans="1:3" s="16" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="36"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="38">
+      <c r="A4" s="42">
         <v>45159</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1264,7 +1280,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
@@ -1273,7 +1289,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="30">
+      <c r="A6" s="40">
         <v>45160</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1284,7 +1300,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="7" t="s">
         <v>2</v>
       </c>
@@ -1293,7 +1309,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
@@ -1302,7 +1318,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="30">
+      <c r="A9" s="40">
         <v>45161</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1313,7 +1329,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
@@ -1322,7 +1338,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="7" t="s">
         <v>16</v>
       </c>
@@ -1331,7 +1347,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="7" t="s">
         <v>17</v>
       </c>
@@ -1340,7 +1356,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="30">
+      <c r="A13" s="40">
         <v>45162</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -1351,7 +1367,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="7" t="s">
         <v>20</v>
       </c>
@@ -1360,7 +1376,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="7" t="s">
         <v>23</v>
       </c>
@@ -1369,7 +1385,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="7" t="s">
         <v>25</v>
       </c>
@@ -1378,7 +1394,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="30">
+      <c r="A17" s="40">
         <v>45163</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -1389,7 +1405,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="7" t="s">
         <v>30</v>
       </c>
@@ -1398,7 +1414,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="7" t="s">
         <v>4</v>
       </c>
@@ -1407,7 +1423,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="7" t="s">
         <v>32</v>
       </c>
@@ -1438,15 +1454,15 @@
       </c>
     </row>
     <row r="23" spans="1:4" s="17" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="36"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="31"/>
       <c r="D23" s="21"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="30">
+      <c r="A24" s="40">
         <v>45166</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -1457,7 +1473,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="10" t="s">
         <v>41</v>
       </c>
@@ -1466,7 +1482,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
+      <c r="A26" s="40"/>
       <c r="B26" s="10" t="s">
         <v>42</v>
       </c>
@@ -1475,7 +1491,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="7" t="s">
         <v>43</v>
       </c>
@@ -1484,7 +1500,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="7" t="s">
         <v>46</v>
       </c>
@@ -1493,7 +1509,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="7" t="s">
         <v>48</v>
       </c>
@@ -1502,7 +1518,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="30">
+      <c r="A30" s="40">
         <v>45167</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -1513,7 +1529,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="7" t="s">
         <v>52</v>
       </c>
@@ -1522,7 +1538,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="7" t="s">
         <v>55</v>
       </c>
@@ -1531,7 +1547,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="30">
+      <c r="A33" s="40">
         <v>45168</v>
       </c>
       <c r="B33" s="7" t="s">
@@ -1542,7 +1558,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
+      <c r="A34" s="40"/>
       <c r="B34" s="7" t="s">
         <v>56</v>
       </c>
@@ -1551,7 +1567,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
+      <c r="A35" s="40"/>
       <c r="B35" s="7" t="s">
         <v>58</v>
       </c>
@@ -1560,7 +1576,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
+      <c r="A36" s="40"/>
       <c r="B36" s="7" t="s">
         <v>61</v>
       </c>
@@ -1602,7 +1618,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="30">
+      <c r="A40" s="40">
         <v>45172</v>
       </c>
       <c r="B40" s="7" t="s">
@@ -1613,7 +1629,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
+      <c r="A41" s="40"/>
       <c r="B41" s="7" t="s">
         <v>70</v>
       </c>
@@ -1622,7 +1638,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="30"/>
+      <c r="A42" s="40"/>
       <c r="B42" s="7" t="s">
         <v>71</v>
       </c>
@@ -1631,15 +1647,15 @@
       </c>
     </row>
     <row r="43" spans="1:4" s="17" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="B43" s="35"/>
-      <c r="C43" s="36"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="31"/>
       <c r="D43" s="21"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="30">
+      <c r="A44" s="40">
         <v>45173</v>
       </c>
       <c r="B44" s="7" t="s">
@@ -1650,7 +1666,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
+      <c r="A45" s="40"/>
       <c r="B45" s="7" t="s">
         <v>2</v>
       </c>
@@ -1659,7 +1675,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
+      <c r="A46" s="40"/>
       <c r="B46" s="10" t="s">
         <v>75</v>
       </c>
@@ -1668,7 +1684,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="30"/>
+      <c r="A47" s="40"/>
       <c r="B47" s="7" t="s">
         <v>77</v>
       </c>
@@ -1677,7 +1693,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
+      <c r="A48" s="40"/>
       <c r="B48" s="7" t="s">
         <v>79</v>
       </c>
@@ -1686,25 +1702,25 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="30">
+      <c r="A49" s="40">
         <v>45174</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="29" t="s">
+      <c r="C49" s="41" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="30"/>
+      <c r="A50" s="40"/>
       <c r="B50" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C50" s="29"/>
+      <c r="C50" s="41"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="30">
+      <c r="A51" s="40">
         <v>45175</v>
       </c>
       <c r="B51" s="7" t="s">
@@ -1715,7 +1731,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="30"/>
+      <c r="A52" s="40"/>
       <c r="B52" s="7" t="s">
         <v>86</v>
       </c>
@@ -1724,7 +1740,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
+      <c r="A53" s="40"/>
       <c r="B53" s="7" t="s">
         <v>88</v>
       </c>
@@ -1733,25 +1749,25 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="30">
+      <c r="A54" s="40">
         <v>45176</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C54" s="29" t="s">
+      <c r="C54" s="41" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
+      <c r="A55" s="40"/>
       <c r="B55" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C55" s="29"/>
+      <c r="C55" s="41"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="30"/>
+      <c r="A56" s="40"/>
       <c r="B56" s="7" t="s">
         <v>91</v>
       </c>
@@ -1760,7 +1776,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="30">
+      <c r="A57" s="40">
         <v>45177</v>
       </c>
       <c r="B57" s="7" t="s">
@@ -1771,7 +1787,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="30"/>
+      <c r="A58" s="40"/>
       <c r="B58" s="7" t="s">
         <v>94</v>
       </c>
@@ -1780,7 +1796,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="30"/>
+      <c r="A59" s="40"/>
       <c r="B59" s="7" t="s">
         <v>95</v>
       </c>
@@ -1789,33 +1805,33 @@
       </c>
     </row>
     <row r="60" spans="1:4" s="17" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="34" t="s">
+      <c r="A60" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="B60" s="35"/>
-      <c r="C60" s="36"/>
+      <c r="B60" s="30"/>
+      <c r="C60" s="31"/>
       <c r="D60" s="21"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="30">
+      <c r="A61" s="40">
         <v>45180</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C61" s="29" t="s">
+      <c r="C61" s="41" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
+      <c r="A62" s="40"/>
       <c r="B62" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C62" s="29"/>
+      <c r="C62" s="41"/>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="30">
+      <c r="A63" s="40">
         <v>45181</v>
       </c>
       <c r="B63" s="7" t="s">
@@ -1826,8 +1842,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="30"/>
-      <c r="B64" s="31" t="s">
+      <c r="A64" s="40"/>
+      <c r="B64" s="43" t="s">
         <v>101</v>
       </c>
       <c r="C64" s="14" t="s">
@@ -1835,98 +1851,98 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="30"/>
-      <c r="B65" s="31"/>
+      <c r="A65" s="40"/>
+      <c r="B65" s="43"/>
       <c r="C65" s="14" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="30"/>
-      <c r="B66" s="31"/>
+      <c r="A66" s="40"/>
+      <c r="B66" s="43"/>
       <c r="C66" s="14" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="33"/>
-      <c r="B67" s="32"/>
+      <c r="A67" s="45"/>
+      <c r="B67" s="44"/>
       <c r="C67" s="23" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="43">
+      <c r="A68" s="36">
         <v>45182</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C68" s="39" t="s">
-        <v>117</v>
+      <c r="C68" s="32" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="44"/>
+      <c r="A69" s="37"/>
       <c r="B69" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C69" s="40"/>
+      <c r="C69" s="33"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="45"/>
+      <c r="A70" s="38"/>
       <c r="B70" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C70" s="25" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="43">
+      <c r="A71" s="36">
         <v>45183</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C71" s="41" t="s">
-        <v>118</v>
+      <c r="C71" s="34" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="45"/>
+      <c r="A72" s="38"/>
       <c r="B72" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C72" s="42"/>
+      <c r="C72" s="35"/>
     </row>
     <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="43">
+      <c r="A73" s="36">
         <v>45184</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>97</v>
       </c>
       <c r="C73" s="24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="37"/>
+      <c r="B74" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C74" s="24" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="44"/>
-      <c r="B74" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C74" s="24" t="s">
-        <v>122</v>
-      </c>
-    </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="45"/>
+      <c r="A75" s="38"/>
       <c r="B75" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C75" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1941,18 +1957,18 @@
         <v>45186</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C77" s="24" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="17" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="B78" s="35"/>
-      <c r="C78" s="36"/>
+      <c r="A78" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B78" s="30"/>
+      <c r="C78" s="31"/>
       <c r="D78" s="21"/>
     </row>
     <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1960,10 +1976,10 @@
         <v>45187</v>
       </c>
       <c r="B79" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C79" s="24" t="s">
         <v>124</v>
-      </c>
-      <c r="C79" s="24" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1974,7 +1990,7 @@
         <v>63</v>
       </c>
       <c r="C80" s="24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1982,10 +1998,10 @@
         <v>45189</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C81" s="24" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1996,144 +2012,94 @@
         <v>63</v>
       </c>
       <c r="C82" s="24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="22">
         <v>45191</v>
       </c>
-      <c r="B83" s="7"/>
-      <c r="C83" s="24"/>
+      <c r="B83" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C83" s="24" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="22">
         <v>45192</v>
       </c>
-      <c r="B84" s="7"/>
-      <c r="C84" s="24"/>
+      <c r="B84" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C84" s="24" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="85" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="22">
         <v>45193</v>
       </c>
-      <c r="B85" s="7"/>
-      <c r="C85" s="24"/>
+      <c r="B85" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C85" s="24" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="86" spans="1:4" s="17" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="B86" s="35"/>
-      <c r="C86" s="36"/>
+      <c r="A86" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B86" s="30"/>
+      <c r="C86" s="31"/>
       <c r="D86" s="21"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="22">
         <v>45194</v>
       </c>
-      <c r="B87" s="7"/>
-      <c r="C87" s="24"/>
+      <c r="B87" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C87" s="24" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="26">
         <v>45195</v>
       </c>
-      <c r="B88" s="27"/>
-      <c r="C88" s="28" t="s">
-        <v>127</v>
+      <c r="B88" s="47">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C88" s="27" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="26">
         <v>45196</v>
       </c>
-      <c r="B89" s="27"/>
-      <c r="C89" s="28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="22">
-        <v>45197</v>
-      </c>
-      <c r="B90" s="7"/>
-      <c r="C90" s="24"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="22">
-        <v>45198</v>
-      </c>
-      <c r="B91" s="7"/>
-      <c r="C91" s="24"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="22">
-        <v>45199</v>
-      </c>
-      <c r="B92" s="7"/>
-      <c r="C92" s="24"/>
-    </row>
-    <row r="93" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="22">
-        <v>45200</v>
-      </c>
-      <c r="B93" s="7"/>
-      <c r="C93" s="24"/>
-    </row>
-    <row r="94" spans="1:4" s="17" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="B94" s="35"/>
-      <c r="C94" s="36"/>
-      <c r="D94" s="21"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="22">
-        <v>45201</v>
-      </c>
-      <c r="B95" s="7"/>
-      <c r="C95" s="24"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="22">
-        <v>45202</v>
-      </c>
-      <c r="B96" s="7"/>
-      <c r="C96" s="24"/>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="26">
-        <v>45203</v>
-      </c>
-      <c r="B97" s="27"/>
-      <c r="C97" s="28"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="26">
-        <v>45204</v>
-      </c>
-      <c r="B98" s="27"/>
-      <c r="C98" s="28"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="26">
-        <v>45205</v>
-      </c>
-      <c r="B99" s="27"/>
-      <c r="C99" s="28"/>
+      <c r="B89" s="47">
+        <v>0.6875</v>
+      </c>
+      <c r="C89" s="27" t="s">
+        <v>126</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="A94:C94"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="A73:A75"/>
+  <mergeCells count="32">
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="A63:A67"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A60:C60"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A57:A59"/>
     <mergeCell ref="A51:A53"/>
@@ -2150,15 +2116,13 @@
     <mergeCell ref="A24:A29"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="A63:A67"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="A73:A75"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.98425196850393704" right="0.98425196850393704" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2171,7 +2135,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00BA6A5C-AF25-424D-BFE8-5BB7F55B08D1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A62"/>
   <sheetViews>
     <sheetView topLeftCell="A54" workbookViewId="0">

</xml_diff>